<commit_message>
NewParameterInterface With tag and interactions (V0.1)
</commit_message>
<xml_diff>
--- a/SettingsDB.xlsx
+++ b/SettingsDB.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\MATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valentin\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="14130" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="14136" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -389,13 +389,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -424,7 +424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -438,10 +438,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -453,7 +453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -511,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -569,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -598,7 +598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -627,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -656,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -714,7 +714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -801,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -830,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -888,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -946,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -975,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>0</v>
       </c>

</xml_diff>